<commit_message>
Deploy til rot: LMDI - 2beda24b52b3078571421cf68055f15e4eb1cf64
</commit_message>
<xml_diff>
--- a/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.4</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-26T09:37:05+00:00</t>
+    <t>2025-03-18T14:32:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>